<commit_message>
feat: add sprint three artifacts and requirements stack
</commit_message>
<xml_diff>
--- a/documentation/Requirements_Stack.xlsx
+++ b/documentation/Requirements_Stack.xlsx
@@ -3,10 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="r+2GhJvDIrmBcEG3vFk6KGnm2QULOnPQHKGLLGfXL98="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -209,10 +214,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,7 +560,7 @@
       <c r="E9" s="2">
         <v>3.0</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -576,7 +577,7 @@
       <c r="E10" s="2">
         <v>3.0</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -593,7 +594,7 @@
       <c r="E11" s="2">
         <v>5.0</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -610,7 +611,7 @@
       <c r="E12" s="2">
         <v>5.0</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -627,7 +628,7 @@
       <c r="E13" s="2">
         <v>5.0</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -644,7 +645,7 @@
       <c r="E14" s="2">
         <v>5.0</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -661,7 +662,9 @@
       <c r="E15" s="2">
         <v>6.0</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="B16" s="2">
@@ -676,7 +679,9 @@
       <c r="E16" s="2">
         <v>6.0</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="B17" s="2">
@@ -691,7 +696,9 @@
       <c r="E17" s="2">
         <v>6.0</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="B18" s="2">
@@ -706,7 +713,9 @@
       <c r="E18" s="2">
         <v>6.0</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="B19" s="2">
@@ -721,7 +730,9 @@
       <c r="E19" s="2">
         <v>7.0</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="B20" s="2">
@@ -736,7 +747,9 @@
       <c r="E20" s="2">
         <v>7.0</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="B21" s="2">
@@ -751,7 +764,9 @@
       <c r="E21" s="2">
         <v>7.0</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="B22" s="2">
@@ -766,7 +781,9 @@
       <c r="E22" s="2">
         <v>7.0</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="B23" s="2">

</xml_diff>